<commit_message>
updated error messages when valided arg request
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/RP_Searching_Folder_Result.xlsx
+++ b/src/main/resources/templates/RP_Searching_Folder_Result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\st-report\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A79C37-2FCC-49BD-8D2D-98DB919DC0EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A117F6E-C30C-4A1A-94CB-EABAEA9ECFCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4CF732CA-5471-4874-BC8E-8C43436AABB5}"/>
   </bookViews>
@@ -93,47 +93,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>STT</t>
   </si>
   <si>
-    <t>Tên thư mục</t>
-  </si>
-  <si>
-    <t>CN/PGD quản lý tài khoản</t>
-  </si>
-  <si>
-    <t>CN/PGD lưu điện tử</t>
-  </si>
-  <si>
-    <t>Tên nghiệp vụ</t>
-  </si>
-  <si>
-    <t>Mã nghiệp vụ</t>
-  </si>
-  <si>
-    <t>Loại KH</t>
-  </si>
-  <si>
-    <t>Mã KH</t>
-  </si>
-  <si>
-    <t>Tên KH</t>
-  </si>
-  <si>
-    <t>Số CMND/CCCD/KKD</t>
-  </si>
-  <si>
-    <t>Số điện thoại</t>
-  </si>
-  <si>
-    <t>Ngày lưu điện tử</t>
-  </si>
-  <si>
-    <t>KẾT QUẢ TÌM KIẾM THƯ MỤC</t>
-  </si>
-  <si>
     <t>CỘNG HÀO XÃ HỘI CHỦ NGHĨA VIỆT NAM</t>
   </si>
   <si>
@@ -155,46 +119,67 @@
     <t>${it.index}</t>
   </si>
   <si>
-    <t>${it.folderName}</t>
-  </si>
-  <si>
-    <t>${it.cnPgdSaving}</t>
-  </si>
-  <si>
-    <t>${it.cnPgdManager}</t>
-  </si>
-  <si>
-    <t>${it.businessName}</t>
-  </si>
-  <si>
-    <t>${it.businessCode}</t>
-  </si>
-  <si>
-    <t>${it.customerType}</t>
-  </si>
-  <si>
-    <t>${it.customerName}</t>
-  </si>
-  <si>
-    <t>${it.customerCode}</t>
-  </si>
-  <si>
-    <t>${it.identification}</t>
-  </si>
-  <si>
-    <t>${it.mobilePhone}</t>
-  </si>
-  <si>
     <t>${it.createdAt}</t>
+  </si>
+  <si>
+    <t>Mã yêu cầu</t>
+  </si>
+  <si>
+    <t>Mã khách hàng</t>
+  </si>
+  <si>
+    <t>Quy trình</t>
+  </si>
+  <si>
+    <t>Người tạo</t>
+  </si>
+  <si>
+    <t>Đơn vị tạo</t>
+  </si>
+  <si>
+    <t>Thời gian tạo</t>
+  </si>
+  <si>
+    <t>Người xử lý</t>
+  </si>
+  <si>
+    <t>Đơn vị xử lý</t>
+  </si>
+  <si>
+    <t>Trạng thái</t>
+  </si>
+  <si>
+    <t>${it.caseId}</t>
+  </si>
+  <si>
+    <t>${it.customerId}</t>
+  </si>
+  <si>
+    <t>${it.processName}</t>
+  </si>
+  <si>
+    <t>${it.createdBy}</t>
+  </si>
+  <si>
+    <t>${it.createdBranch}</t>
+  </si>
+  <si>
+    <t>${it.creator}</t>
+  </si>
+  <si>
+    <t>${it.branchCreator}</t>
+  </si>
+  <si>
+    <t>${it.status}</t>
+  </si>
+  <si>
+    <t>DANH SÁCH YÊU CẦU</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm"/>
-  </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -286,11 +271,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -299,9 +290,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -617,10 +605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{888862A1-B274-462E-A019-3145F8B971BF}">
-  <dimension ref="B2:M10"/>
+  <dimension ref="B1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,155 +627,153 @@
     <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+    </row>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="J2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
+      <c r="B2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="H2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="J3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
+      <c r="B3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="H3" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="J5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="H4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
+      <c r="B6" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
+      <c r="B7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>11</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="F10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="2" t="s">
+      <c r="H10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="J10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="K10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="M10" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="L10" s="4"/>
+      <c r="M10" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="B6:M6"/>
-    <mergeCell ref="B7:M7"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="J3:M3"/>
-    <mergeCell ref="J5:M5"/>
+    <mergeCell ref="B6:K6"/>
+    <mergeCell ref="B7:K7"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="H4:K4"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B3:D3"/>
   </mergeCells>

</xml_diff>